<commit_message>
added odds ratio column option
</commit_message>
<xml_diff>
--- a/inst/examples/Outputs/summary_oper_vs_nonop.xlsx
+++ b/inst/examples/Outputs/summary_oper_vs_nonop.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,53 +383,58 @@
           <t>test</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>index_group: IR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>33 ± 18.9</t>
+          <t>22 (34%)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>116 ± 29.3</t>
+          <t>0 (0%)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.8e-27</t>
+          <t>9e-48</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Wilcoxon rank-sum</t>
+          <t>Fisher exact</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>index_group: IR</t>
+          <t>index_group: OR_K</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22 (34%)</t>
+          <t>0 (0%)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0 (0%)</t>
+          <t>101 (100%)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8.6e-48</t>
+          <t>9e-48</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -441,22 +446,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>index_group: OR_K</t>
+          <t>index_group: SM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>43 (66%)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>0 (0%)</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>101 (100%)</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8.6e-48</t>
+          <t>9e-48</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -468,211 +473,231 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>index_group: SM</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>43 (66%)</t>
+          <t>3.5 ± 0.5</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0 (0%)</t>
+          <t>4.4 ± 0.5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>8.6e-48</t>
+          <t>1e-18</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fisher exact</t>
+          <t>Wilcoxon rank-sum</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>grade</t>
+          <t>survived: Y</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.5 ± 0.5</t>
+          <t>63 (97%)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.4 ± 0.5</t>
+          <t>87 (86%)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.1e-18</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Wilcoxon rank-sum</t>
+          <t>Fisher exact</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.20 [0.04–0.90]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>survived: Y</t>
+          <t>renal_pres: Y</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>63 (97%)</t>
+          <t>65 (100%)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>87 (86%)</t>
+          <t>36 (36%)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.029</t>
+          <t>3e-20</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>Fisher exact</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.00 [0.00–NaN]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>renal_pres: Y</t>
+          <t>AKI: Y</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>65 (100%)</t>
+          <t>15 (24%)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>36 (36%)</t>
+          <t>39 (45%)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.8e-20</t>
+          <t>0.013</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Fisher exact</t>
+          <t>Chi-squared</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2.60 [1.27–5.33]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AKI: Y</t>
+          <t>return_ed_30d: Y</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16 (25%)</t>
+          <t>17 (27%)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>46 (46%)</t>
+          <t>30 (34%)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.011</t>
+          <t>0.42</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>Chi-squared</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1.42 [0.70–2.90]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>return_ed_30d: Y</t>
+          <t>GCS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18 (28%)</t>
+          <t>14 [12–16]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>33 (33%)</t>
+          <t>13 [10–16]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>0.062</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Chi-squared</t>
+          <t>Wilcoxon rank-sum</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GCS</t>
+          <t>ED_SBP</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>14 [12–16]</t>
+          <t>118.6 ± 35.5</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13 [10–16]</t>
+          <t>114.6 ± 29.9</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.062</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Wilcoxon rank-sum</t>
+          <t>Welch t-test</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ED_SBP</t>
+          <t>ED_DBP</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>118.6 ± 35.5</t>
+          <t>72.4 ± 30.6</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>114.6 ± 29.9</t>
+          <t>66.7 ± 20.2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -684,22 +709,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ED_DBP</t>
+          <t>MAP_calc</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>72.4 ± 30.6</t>
+          <t>85 ± 27.4</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>66.7 ± 20.2</t>
+          <t>85.9 ± 24.8</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.18</t>
+          <t>0.83</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -711,49 +736,49 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MAP_calc</t>
+          <t>ED_HR</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>85 ± 27.4</t>
+          <t>98.3 ± 29.6</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>85.9 ± 24.8</t>
+          <t>96.4 ± 29.9</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.83</t>
+          <t>0.54</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Welch t-test</t>
+          <t>Wilcoxon rank-sum</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ED_HR</t>
+          <t>ISS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>98.3 ± 29.6</t>
+          <t>26 [20–33]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>96.4 ± 29.9</t>
+          <t>30 [22–35]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.54</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -765,22 +790,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ISS</t>
+          <t>surv_ICU_LOS</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>26 [20–33]</t>
+          <t>6.3 ± 3.3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>30 [22–35]</t>
+          <t>11.3 ± 7.8</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>3e-04</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -792,22 +817,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>surv_ICU_LOS</t>
+          <t>vent_LOS</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6.3 ± 3.3</t>
+          <t>6.8 ± 3.8</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>11.3 ± 7.8</t>
+          <t>9.6 ± 5.7</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3.5e-04</t>
+          <t>0.005</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -819,22 +844,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>vent_LOS</t>
+          <t>surv_hosp_LOS</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6.8 ± 3.8</t>
+          <t>17.1 ± 9.9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>9.6 ± 5.7</t>
+          <t>29.2 ± 18.2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.005</t>
+          <t>5e-05</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -846,79 +871,52 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>surv_hosp_LOS</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17.1 ± 9.9</t>
+          <t>26.5 ± 9</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>29.2 ± 18.2</t>
+          <t>29.8 ± 12</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4.8e-05</t>
+          <t>0.046</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Wilcoxon rank-sum</t>
+          <t>Welch t-test</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>BMI</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>26.5 ± 9</t>
+          <t>25 ± 5.6</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>29.8 ± 12</t>
+          <t>26.3 ± 6.2</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.046</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
-        <is>
-          <t>Welch t-test</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>BMI</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>25 ± 5.6</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>26.3 ± 6.2</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0.18</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
         <is>
           <t>Welch t-test</t>
         </is>

</xml_diff>